<commit_message>
Remove `"": null` test from example XLSForm
</commit_message>
<xml_diff>
--- a/Example XLSForm.xlsx
+++ b/Example XLSForm.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="choices" sheetId="1" state="visible" r:id="rId2"/>
@@ -417,7 +417,7 @@
     <t xml:space="preserve">state_combined_style</t>
   </si>
   <si>
-    <t xml:space="preserve">concat('{', ${state_instance_style}, '"": null', '}')</t>
+    <t xml:space="preserve">concat('{', ${state_instance_style}, '"selected": { "stroke": "yellow", "stroke-width": "10"}', '}')</t>
   </si>
   <si>
     <t xml:space="preserve">namespaces</t>
@@ -438,6 +438,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -521,8 +522,8 @@
   </sheetPr>
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1145,19 +1146,19 @@
   </sheetPr>
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="38.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="29.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="109.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="109.87"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -1261,7 +1262,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1299,7 +1300,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>